<commit_message>
EPBDS-9443 Automatically determine SpreadsheetResult cell type
--HG--
branch : EPBDS-9443
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7651_sum_object_message.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7651_sum_object_message.xlsx
@@ -1,16 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9E759B-2151-4DA1-9A23-B8305AC41AE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8625" yWindow="1155" windowWidth="23520" windowHeight="10500" tabRatio="823"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" tabRatio="823" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VehiclePremium" sheetId="5" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -70,9 +83,6 @@
     <t>RETURN</t>
   </si>
   <si>
-    <t>= $Rate$TotalCoveragePremium ( $RaterCoverages )</t>
-  </si>
-  <si>
     <t>Totals</t>
   </si>
   <si>
@@ -80,13 +90,16 @@
   </si>
   <si>
     <t>=  CoveragePremiumCalculation (  new String[0] )</t>
+  </si>
+  <si>
+    <t>= (Object[]) $Rate$TotalCoveragePremium ( $RaterCoverages )</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -594,53 +607,54 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% — акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% — акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% — акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% — акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% — акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% — акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% — акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% — акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% — акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% — акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% — акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% — акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% — акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% — акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% — акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% — акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% — акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Акцент4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Акцент5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Акцент6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ввод " xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Вывод" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Вычисление" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Заголовок 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Заголовок 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Заголовок 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Заголовок 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Итог" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Контрольная ячейка" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Название" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Нейтральный" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Пояснение" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Примечание" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Связанная ячейка" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Текст предупреждения" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Хороший" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -648,14 +662,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -693,9 +710,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -728,9 +745,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -763,9 +797,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -938,29 +989,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C14" sqref="C14:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="59.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="119.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="59.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="119.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.3984375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.265625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:4" ht="15.4">
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:4">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -968,47 +1019,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:4">
       <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4">
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:4">
       <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
-        <v>13</v>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:4">
       <c r="C9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:4">
       <c r="C10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:4">
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:4">
       <c r="C15" t="s">
         <v>3</v>
       </c>
@@ -1016,7 +1067,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:4">
       <c r="C16" t="s">
         <v>5</v>
       </c>

</xml_diff>